<commit_message>
updated to OSM-S-105 and data to OSM-S-95
</commit_message>
<xml_diff>
--- a/gdoc_Available OSDD Malaria Compounds.xlsx
+++ b/gdoc_Available OSDD Malaria Compounds.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="680" windowWidth="25360" windowHeight="13180" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="675" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
     <sheet name="Bio tested compounds" sheetId="2" r:id="rId2"/>
     <sheet name="Desired compounds" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="1112">
   <si>
     <t>Compound Identifier</t>
   </si>
@@ -3252,13 +3252,118 @@
   </si>
   <si>
     <t>OSM-S-9</t>
+  </si>
+  <si>
+    <t>OSM-S-96</t>
+  </si>
+  <si>
+    <t>OSM-S-97</t>
+  </si>
+  <si>
+    <t>OSM-S-98</t>
+  </si>
+  <si>
+    <t>OSM-S-99</t>
+  </si>
+  <si>
+    <t>OSM-S-100</t>
+  </si>
+  <si>
+    <t>OSM-S-101</t>
+  </si>
+  <si>
+    <t>OSM-S-102</t>
+  </si>
+  <si>
+    <t>OSM-S-103</t>
+  </si>
+  <si>
+    <t>OSM-S-104</t>
+  </si>
+  <si>
+    <t>OSM-S-105</t>
+  </si>
+  <si>
+    <t>MJT6-1</t>
+  </si>
+  <si>
+    <t>MNR51-1</t>
+  </si>
+  <si>
+    <t>MNR52-1</t>
+  </si>
+  <si>
+    <t>MD17-1</t>
+  </si>
+  <si>
+    <t>MD18-1</t>
+  </si>
+  <si>
+    <t>PMY59-3</t>
+  </si>
+  <si>
+    <t>MNR53-1</t>
+  </si>
+  <si>
+    <t>MNR54-1</t>
+  </si>
+  <si>
+    <t>MNR55-1</t>
+  </si>
+  <si>
+    <t>MNR56-1</t>
+  </si>
+  <si>
+    <t>http://malaria.ourexperiment.org/pyrazole/5099/Cyclodehydration_of_coupled_pyrazole_core_MJT51_and_subsequent_oxidation_to_oxazole_MJT_61.html</t>
+  </si>
+  <si>
+    <t>http://malaria.ourexperiment.org/tcmdc_ap/5189/FriedelsCraft_Acylation_of_AEW11_to_give_MNR511.html</t>
+  </si>
+  <si>
+    <t>http://malaria.ourexperiment.org/tcmdc_ap/5247/EDC_Coupling_of_MNR51_with_Dimethylamine_to_give_MNR521.html</t>
+  </si>
+  <si>
+    <t>http://malaria.ourexperiment.org/tcmdc_ap/5393/EDC_Coupling_of_MNR51_with_methylamine_to_give_MNR531.html</t>
+  </si>
+  <si>
+    <t>http://malaria.ourexperiment.org/tcmdc_ap/5431/EDC_Coupling_of_MNR51_with_Ammonium_Hydroxide_to_give_MNR541.html</t>
+  </si>
+  <si>
+    <t>http://malaria.ourexperiment.org/pyrazole/5445/Hydrolysis_of_MJT61_to_give_MNR551.html</t>
+  </si>
+  <si>
+    <t>http://malaria.ourexperiment.org/pyrazole/5530/EDC_Coupling_of_MNR55_with_Ammonium_Hydroxide_to_give_MNR561.html</t>
+  </si>
+  <si>
+    <t>http://malaria.ourexperiment.org/matind/5671/Synthesis_of_1ethoxy1oxopropan2yl_14fluorophenyl25dimethyl1Hpyrrole3carboxylate_through_ester_synthesis_MD_171.html</t>
+  </si>
+  <si>
+    <t>http://malaria.ourexperiment.org/matind/5746/Hydrolysis_of_MD_171_to_give_214fluorophenyl25dimethyl1Hpyrrole3carbonyloxypropanoic_acid_MD_181.html</t>
+  </si>
+  <si>
+    <t>http://malaria.ourexperiment.org/tcmdc_ap/5097/Hydrolysis_of_PMY_583_methyl_ester_PMY_593.html</t>
+  </si>
+  <si>
+    <t>&gt;100000</t>
+  </si>
+  <si>
+    <t>80% @ 40uM</t>
+  </si>
+  <si>
+    <t>70% @ 40 uM</t>
+  </si>
+  <si>
+    <t>85% @ 40 uM</t>
+  </si>
+  <si>
+    <t>96% @ 40uM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3317,6 +3422,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -3505,10 +3616,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3585,12 +3697,22 @@
     <xf numFmtId="49" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3919,22 +4041,22 @@
   <dimension ref="A1:AM118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="AA104" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="AA101" sqref="AA101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="60">
+    <row r="1" spans="1:39" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4053,7 +4175,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="41.25" customHeight="1">
+    <row r="2" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1068</v>
       </c>
@@ -4122,7 +4244,7 @@
       <c r="AJ2" s="27"/>
       <c r="AK2" s="27"/>
     </row>
-    <row r="3" spans="1:39" ht="41.25" customHeight="1">
+    <row r="3" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1069</v>
       </c>
@@ -4202,7 +4324,7 @@
       <c r="AJ3" s="27"/>
       <c r="AK3" s="27"/>
     </row>
-    <row r="4" spans="1:39" ht="41.25" customHeight="1">
+    <row r="4" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>1070</v>
       </c>
@@ -4289,7 +4411,7 @@
       <c r="AJ4" s="27"/>
       <c r="AK4" s="27"/>
     </row>
-    <row r="5" spans="1:39" ht="41.25" customHeight="1">
+    <row r="5" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>1071</v>
       </c>
@@ -4374,7 +4496,7 @@
       <c r="AJ5" s="27"/>
       <c r="AK5" s="27"/>
     </row>
-    <row r="6" spans="1:39" ht="41.25" customHeight="1">
+    <row r="6" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>1072</v>
       </c>
@@ -4483,7 +4605,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="41.25" customHeight="1">
+    <row r="7" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>1073</v>
       </c>
@@ -4583,7 +4705,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="41.25" customHeight="1">
+    <row r="8" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1074</v>
       </c>
@@ -4666,7 +4788,7 @@
       <c r="AJ8" s="27"/>
       <c r="AK8" s="27"/>
     </row>
-    <row r="9" spans="1:39" ht="41.25" customHeight="1">
+    <row r="9" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1075</v>
       </c>
@@ -4742,7 +4864,7 @@
       <c r="AJ9" s="27"/>
       <c r="AK9" s="27"/>
     </row>
-    <row r="10" spans="1:39" ht="41.25" customHeight="1">
+    <row r="10" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>1076</v>
       </c>
@@ -4839,7 +4961,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="41.25" customHeight="1">
+    <row r="11" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>141</v>
       </c>
@@ -4938,7 +5060,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="41.25" customHeight="1">
+    <row r="12" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>158</v>
       </c>
@@ -5005,7 +5127,7 @@
       <c r="AJ12" s="27"/>
       <c r="AK12" s="27"/>
     </row>
-    <row r="13" spans="1:39" ht="41.25" customHeight="1">
+    <row r="13" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>167</v>
       </c>
@@ -5080,7 +5202,7 @@
       <c r="AJ13" s="27"/>
       <c r="AK13" s="27"/>
     </row>
-    <row r="14" spans="1:39" ht="41.25" customHeight="1">
+    <row r="14" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>180</v>
       </c>
@@ -5153,7 +5275,7 @@
       <c r="AJ14" s="27"/>
       <c r="AK14" s="27"/>
     </row>
-    <row r="15" spans="1:39" ht="41.25" customHeight="1">
+    <row r="15" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>191</v>
       </c>
@@ -5226,7 +5348,7 @@
       <c r="AJ15" s="27"/>
       <c r="AK15" s="27"/>
     </row>
-    <row r="16" spans="1:39" ht="41.25" customHeight="1">
+    <row r="16" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>200</v>
       </c>
@@ -5289,7 +5411,7 @@
       <c r="AJ16" s="27"/>
       <c r="AK16" s="27"/>
     </row>
-    <row r="17" spans="1:37" ht="41.25" customHeight="1">
+    <row r="17" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
         <v>209</v>
       </c>
@@ -5366,7 +5488,7 @@
       <c r="AJ17" s="27"/>
       <c r="AK17" s="27"/>
     </row>
-    <row r="18" spans="1:37" ht="41.25" customHeight="1">
+    <row r="18" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>220</v>
       </c>
@@ -5429,7 +5551,7 @@
       <c r="AJ18" s="27"/>
       <c r="AK18" s="27"/>
     </row>
-    <row r="19" spans="1:37" ht="41.25" customHeight="1">
+    <row r="19" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>228</v>
       </c>
@@ -5490,7 +5612,7 @@
       <c r="AJ19" s="27"/>
       <c r="AK19" s="27"/>
     </row>
-    <row r="20" spans="1:37" ht="41.25" customHeight="1">
+    <row r="20" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
         <v>237</v>
       </c>
@@ -5569,7 +5691,7 @@
       <c r="AJ20" s="27"/>
       <c r="AK20" s="27"/>
     </row>
-    <row r="21" spans="1:37" ht="41.25" customHeight="1">
+    <row r="21" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>246</v>
       </c>
@@ -5630,7 +5752,7 @@
       <c r="AJ21" s="27"/>
       <c r="AK21" s="27"/>
     </row>
-    <row r="22" spans="1:37" ht="41.25" customHeight="1">
+    <row r="22" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>254</v>
       </c>
@@ -5704,7 +5826,7 @@
       <c r="AJ22" s="27"/>
       <c r="AK22" s="27"/>
     </row>
-    <row r="23" spans="1:37" ht="41.25" customHeight="1">
+    <row r="23" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>264</v>
       </c>
@@ -5765,7 +5887,7 @@
       <c r="AJ23" s="27"/>
       <c r="AK23" s="27"/>
     </row>
-    <row r="24" spans="1:37" ht="41.25" customHeight="1">
+    <row r="24" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>270</v>
       </c>
@@ -5830,7 +5952,7 @@
       <c r="AJ24" s="27"/>
       <c r="AK24" s="27"/>
     </row>
-    <row r="25" spans="1:37" ht="41.25" customHeight="1">
+    <row r="25" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>280</v>
       </c>
@@ -5899,7 +6021,7 @@
       <c r="AJ25" s="27"/>
       <c r="AK25" s="27"/>
     </row>
-    <row r="26" spans="1:37" ht="41.25" customHeight="1">
+    <row r="26" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>289</v>
       </c>
@@ -5968,7 +6090,7 @@
       <c r="AJ26" s="27"/>
       <c r="AK26" s="27"/>
     </row>
-    <row r="27" spans="1:37" ht="41.25" customHeight="1">
+    <row r="27" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>300</v>
       </c>
@@ -6035,7 +6157,7 @@
       <c r="AJ27" s="27"/>
       <c r="AK27" s="27"/>
     </row>
-    <row r="28" spans="1:37" ht="41.25" customHeight="1">
+    <row r="28" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>308</v>
       </c>
@@ -6097,7 +6219,7 @@
       <c r="AJ28" s="27"/>
       <c r="AK28" s="27"/>
     </row>
-    <row r="29" spans="1:37" ht="41.25" customHeight="1">
+    <row r="29" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>316</v>
       </c>
@@ -6173,7 +6295,7 @@
       <c r="AJ29" s="27"/>
       <c r="AK29" s="27"/>
     </row>
-    <row r="30" spans="1:37" ht="41.25" customHeight="1">
+    <row r="30" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>328</v>
       </c>
@@ -6249,7 +6371,7 @@
       <c r="AJ30" s="27"/>
       <c r="AK30" s="27"/>
     </row>
-    <row r="31" spans="1:37" ht="41.25" customHeight="1">
+    <row r="31" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>339</v>
       </c>
@@ -6327,7 +6449,7 @@
       <c r="AJ31" s="27"/>
       <c r="AK31" s="27"/>
     </row>
-    <row r="32" spans="1:37" ht="41.25" customHeight="1">
+    <row r="32" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>351</v>
       </c>
@@ -6405,7 +6527,7 @@
       <c r="AJ32" s="27"/>
       <c r="AK32" s="27"/>
     </row>
-    <row r="33" spans="1:39" ht="41.25" customHeight="1">
+    <row r="33" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>364</v>
       </c>
@@ -6481,7 +6603,7 @@
       <c r="AJ33" s="27"/>
       <c r="AK33" s="27"/>
     </row>
-    <row r="34" spans="1:39" ht="41.25" customHeight="1">
+    <row r="34" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
         <v>375</v>
       </c>
@@ -6558,7 +6680,7 @@
       <c r="AJ34" s="27"/>
       <c r="AK34" s="27"/>
     </row>
-    <row r="35" spans="1:39" ht="41.25" customHeight="1">
+    <row r="35" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>387</v>
       </c>
@@ -6634,7 +6756,7 @@
       <c r="AJ35" s="27"/>
       <c r="AK35" s="27"/>
     </row>
-    <row r="36" spans="1:39" ht="41.25" customHeight="1">
+    <row r="36" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>400</v>
       </c>
@@ -6731,7 +6853,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:39" ht="41.25" customHeight="1">
+    <row r="37" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
         <v>413</v>
       </c>
@@ -6808,7 +6930,7 @@
       <c r="AJ37" s="27"/>
       <c r="AK37" s="27"/>
     </row>
-    <row r="38" spans="1:39" ht="41.25" customHeight="1">
+    <row r="38" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>423</v>
       </c>
@@ -6901,7 +7023,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="39" spans="1:39" ht="41.25" customHeight="1">
+    <row r="39" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="25" t="s">
         <v>433</v>
       </c>
@@ -6996,7 +7118,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="40" spans="1:39" ht="41.25" customHeight="1">
+    <row r="40" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>446</v>
       </c>
@@ -7089,7 +7211,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="41" spans="1:39" ht="41.25" customHeight="1">
+    <row r="41" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>456</v>
       </c>
@@ -7165,7 +7287,7 @@
       <c r="AJ41" s="27"/>
       <c r="AK41" s="27"/>
     </row>
-    <row r="42" spans="1:39" ht="41.25" customHeight="1">
+    <row r="42" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>467</v>
       </c>
@@ -7237,7 +7359,7 @@
       <c r="AJ42" s="27"/>
       <c r="AK42" s="27"/>
     </row>
-    <row r="43" spans="1:39" ht="41.25" customHeight="1">
+    <row r="43" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>476</v>
       </c>
@@ -7319,7 +7441,7 @@
       <c r="AJ43" s="27"/>
       <c r="AK43" s="27"/>
     </row>
-    <row r="44" spans="1:39" ht="41.25" customHeight="1">
+    <row r="44" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>488</v>
       </c>
@@ -7399,7 +7521,7 @@
       <c r="AJ44" s="27"/>
       <c r="AK44" s="27"/>
     </row>
-    <row r="45" spans="1:39" ht="41.25" customHeight="1">
+    <row r="45" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>495</v>
       </c>
@@ -7471,7 +7593,7 @@
       <c r="AJ45" s="27"/>
       <c r="AK45" s="27"/>
     </row>
-    <row r="46" spans="1:39" ht="41.25" customHeight="1">
+    <row r="46" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="25" t="s">
         <v>505</v>
       </c>
@@ -7548,7 +7670,7 @@
       <c r="AJ46" s="27"/>
       <c r="AK46" s="27"/>
     </row>
-    <row r="47" spans="1:39" ht="41.25" customHeight="1">
+    <row r="47" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>513</v>
       </c>
@@ -7622,7 +7744,7 @@
       <c r="AJ47" s="27"/>
       <c r="AK47" s="27"/>
     </row>
-    <row r="48" spans="1:39" ht="41.25" customHeight="1">
+    <row r="48" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>523</v>
       </c>
@@ -7696,7 +7818,7 @@
       <c r="AJ48" s="27"/>
       <c r="AK48" s="27"/>
     </row>
-    <row r="49" spans="1:37" ht="41.25" customHeight="1">
+    <row r="49" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>535</v>
       </c>
@@ -7779,7 +7901,7 @@
       <c r="AJ49" s="27"/>
       <c r="AK49" s="27"/>
     </row>
-    <row r="50" spans="1:37" ht="41.25" customHeight="1">
+    <row r="50" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>547</v>
       </c>
@@ -7858,7 +7980,7 @@
       <c r="AJ50" s="27"/>
       <c r="AK50" s="27"/>
     </row>
-    <row r="51" spans="1:37" ht="41.25" customHeight="1">
+    <row r="51" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>555</v>
       </c>
@@ -7935,7 +8057,7 @@
       <c r="AJ51" s="27"/>
       <c r="AK51" s="27"/>
     </row>
-    <row r="52" spans="1:37" ht="41.25" customHeight="1">
+    <row r="52" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>563</v>
       </c>
@@ -8014,7 +8136,7 @@
       <c r="AJ52" s="27"/>
       <c r="AK52" s="27"/>
     </row>
-    <row r="53" spans="1:37" ht="41.25" customHeight="1">
+    <row r="53" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>573</v>
       </c>
@@ -8095,7 +8217,7 @@
       <c r="AJ53" s="27"/>
       <c r="AK53" s="27"/>
     </row>
-    <row r="54" spans="1:37" ht="41.25" customHeight="1">
+    <row r="54" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>582</v>
       </c>
@@ -8165,7 +8287,7 @@
       <c r="AJ54" s="27"/>
       <c r="AK54" s="27"/>
     </row>
-    <row r="55" spans="1:37" ht="41.25" customHeight="1">
+    <row r="55" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>592</v>
       </c>
@@ -8258,7 +8380,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="41.25" customHeight="1">
+    <row r="56" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="25" t="s">
         <v>600</v>
       </c>
@@ -8337,7 +8459,7 @@
       <c r="AJ56" s="27"/>
       <c r="AK56" s="27"/>
     </row>
-    <row r="57" spans="1:37" ht="41.25" customHeight="1">
+    <row r="57" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>611</v>
       </c>
@@ -8400,7 +8522,9 @@
       <c r="Z57" t="s">
         <v>622</v>
       </c>
-      <c r="AA57" s="5"/>
+      <c r="AA57" s="5">
+        <v>333</v>
+      </c>
       <c r="AB57" s="31"/>
       <c r="AC57" s="32"/>
       <c r="AD57" s="4"/>
@@ -8412,7 +8536,7 @@
       <c r="AJ57" s="27"/>
       <c r="AK57" s="27"/>
     </row>
-    <row r="58" spans="1:37" ht="41.25" customHeight="1">
+    <row r="58" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>623</v>
       </c>
@@ -8462,7 +8586,9 @@
       <c r="Z58">
         <v>0.81</v>
       </c>
-      <c r="AA58" s="5"/>
+      <c r="AA58" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB58" s="31"/>
       <c r="AC58" s="32"/>
       <c r="AD58" s="4"/>
@@ -8474,7 +8600,7 @@
       <c r="AJ58" s="27"/>
       <c r="AK58" s="27"/>
     </row>
-    <row r="59" spans="1:37" ht="41.25" customHeight="1">
+    <row r="59" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>631</v>
       </c>
@@ -8500,7 +8626,9 @@
       <c r="W59" s="26"/>
       <c r="X59" s="9"/>
       <c r="Y59" s="9"/>
-      <c r="AA59" s="5"/>
+      <c r="AA59" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB59" s="31"/>
       <c r="AC59" s="32"/>
       <c r="AD59" s="4"/>
@@ -8512,7 +8640,7 @@
       <c r="AJ59" s="27"/>
       <c r="AK59" s="27"/>
     </row>
-    <row r="60" spans="1:37" ht="41.25" customHeight="1">
+    <row r="60" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>634</v>
       </c>
@@ -8538,7 +8666,9 @@
       <c r="W60" s="26"/>
       <c r="X60" s="9"/>
       <c r="Y60" s="9"/>
-      <c r="AA60" s="5"/>
+      <c r="AA60" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB60" s="31"/>
       <c r="AC60" s="32"/>
       <c r="AD60" s="4"/>
@@ -8550,7 +8680,7 @@
       <c r="AJ60" s="27"/>
       <c r="AK60" s="27"/>
     </row>
-    <row r="61" spans="1:37" ht="41.25" customHeight="1">
+    <row r="61" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>637</v>
       </c>
@@ -8576,7 +8706,9 @@
       <c r="W61" s="26"/>
       <c r="X61" s="9"/>
       <c r="Y61" s="9"/>
-      <c r="AA61" s="5"/>
+      <c r="AA61" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB61" s="31"/>
       <c r="AC61" s="32"/>
       <c r="AD61" s="4"/>
@@ -8588,7 +8720,7 @@
       <c r="AJ61" s="27"/>
       <c r="AK61" s="27"/>
     </row>
-    <row r="62" spans="1:37" ht="41.25" customHeight="1">
+    <row r="62" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>640</v>
       </c>
@@ -8614,7 +8746,9 @@
       <c r="W62" s="26"/>
       <c r="X62" s="9"/>
       <c r="Y62" s="9"/>
-      <c r="AA62" s="5"/>
+      <c r="AA62" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB62" s="31"/>
       <c r="AC62" s="32"/>
       <c r="AD62" s="4"/>
@@ -8626,7 +8760,7 @@
       <c r="AJ62" s="27"/>
       <c r="AK62" s="27"/>
     </row>
-    <row r="63" spans="1:37" ht="41.25" customHeight="1">
+    <row r="63" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>643</v>
       </c>
@@ -8652,7 +8786,9 @@
       <c r="W63" s="26"/>
       <c r="X63" s="9"/>
       <c r="Y63" s="9"/>
-      <c r="AA63" s="5"/>
+      <c r="AA63" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB63" s="31"/>
       <c r="AC63" s="32"/>
       <c r="AD63" s="4"/>
@@ -8664,7 +8800,7 @@
       <c r="AJ63" s="27"/>
       <c r="AK63" s="27"/>
     </row>
-    <row r="64" spans="1:37" ht="41.25" customHeight="1">
+    <row r="64" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>646</v>
       </c>
@@ -8688,7 +8824,9 @@
       <c r="W64" s="26"/>
       <c r="X64" s="9"/>
       <c r="Y64" s="9"/>
-      <c r="AA64" s="5"/>
+      <c r="AA64" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB64" s="31"/>
       <c r="AC64" s="32"/>
       <c r="AD64" s="4"/>
@@ -8700,7 +8838,7 @@
       <c r="AJ64" s="27"/>
       <c r="AK64" s="27"/>
     </row>
-    <row r="65" spans="1:37" ht="41.25" customHeight="1">
+    <row r="65" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>648</v>
       </c>
@@ -8728,7 +8866,9 @@
       <c r="W65" s="26"/>
       <c r="X65" s="9"/>
       <c r="Y65" s="9"/>
-      <c r="AA65" s="5"/>
+      <c r="AA65" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB65" s="31"/>
       <c r="AC65" s="32"/>
       <c r="AD65" s="4"/>
@@ -8740,7 +8880,7 @@
       <c r="AJ65" s="27"/>
       <c r="AK65" s="27"/>
     </row>
-    <row r="66" spans="1:37" ht="41.25" customHeight="1">
+    <row r="66" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>651</v>
       </c>
@@ -8776,7 +8916,7 @@
       <c r="AJ66" s="27"/>
       <c r="AK66" s="27"/>
     </row>
-    <row r="67" spans="1:37" ht="41.25" customHeight="1">
+    <row r="67" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>653</v>
       </c>
@@ -8804,7 +8944,9 @@
       <c r="W67" s="26"/>
       <c r="X67" s="9"/>
       <c r="Y67" s="9"/>
-      <c r="AA67" s="5"/>
+      <c r="AA67" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB67" s="31"/>
       <c r="AC67" s="32"/>
       <c r="AD67" s="4"/>
@@ -8816,7 +8958,7 @@
       <c r="AJ67" s="27"/>
       <c r="AK67" s="27"/>
     </row>
-    <row r="68" spans="1:37" ht="41.25" customHeight="1">
+    <row r="68" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>656</v>
       </c>
@@ -8844,7 +8986,9 @@
       <c r="W68" s="26"/>
       <c r="X68" s="9"/>
       <c r="Y68" s="9"/>
-      <c r="AA68" s="5"/>
+      <c r="AA68" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB68" s="31"/>
       <c r="AC68" s="32"/>
       <c r="AD68" s="4"/>
@@ -8856,7 +9000,7 @@
       <c r="AJ68" s="27"/>
       <c r="AK68" s="27"/>
     </row>
-    <row r="69" spans="1:37" ht="41.25" customHeight="1">
+    <row r="69" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>659</v>
       </c>
@@ -8884,7 +9028,9 @@
       <c r="W69" s="26"/>
       <c r="X69" s="9"/>
       <c r="Y69" s="9"/>
-      <c r="AA69" s="5"/>
+      <c r="AA69" s="5">
+        <v>438</v>
+      </c>
       <c r="AB69" s="31"/>
       <c r="AC69" s="32"/>
       <c r="AD69" s="4"/>
@@ -8896,7 +9042,7 @@
       <c r="AJ69" s="27"/>
       <c r="AK69" s="27"/>
     </row>
-    <row r="70" spans="1:37" ht="41.25" customHeight="1">
+    <row r="70" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>662</v>
       </c>
@@ -8930,7 +9076,9 @@
       <c r="W70" s="26"/>
       <c r="X70" s="9"/>
       <c r="Y70" s="9"/>
-      <c r="AA70" s="5"/>
+      <c r="AA70" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB70" s="31"/>
       <c r="AC70" s="32"/>
       <c r="AD70" s="4"/>
@@ -8942,7 +9090,7 @@
       <c r="AJ70" s="27"/>
       <c r="AK70" s="27"/>
     </row>
-    <row r="71" spans="1:37" ht="41.25" customHeight="1">
+    <row r="71" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>667</v>
       </c>
@@ -8966,7 +9114,9 @@
       <c r="W71" s="26"/>
       <c r="X71" s="9"/>
       <c r="Y71" s="9"/>
-      <c r="AA71" s="5"/>
+      <c r="AA71" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB71" s="31"/>
       <c r="AC71" s="32"/>
       <c r="AD71" s="4"/>
@@ -8978,7 +9128,7 @@
       <c r="AJ71" s="27"/>
       <c r="AK71" s="27"/>
     </row>
-    <row r="72" spans="1:37" ht="41.25" customHeight="1">
+    <row r="72" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>669</v>
       </c>
@@ -9002,7 +9152,9 @@
       <c r="W72" s="26"/>
       <c r="X72" s="9"/>
       <c r="Y72" s="9"/>
-      <c r="AA72" s="5"/>
+      <c r="AA72" s="35">
+        <v>9400</v>
+      </c>
       <c r="AB72" s="31"/>
       <c r="AC72" s="32"/>
       <c r="AD72" s="4"/>
@@ -9014,7 +9166,7 @@
       <c r="AJ72" s="27"/>
       <c r="AK72" s="27"/>
     </row>
-    <row r="73" spans="1:37" ht="41.25" customHeight="1">
+    <row r="73" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>671</v>
       </c>
@@ -9038,7 +9190,9 @@
       <c r="W73" s="26"/>
       <c r="X73" s="9"/>
       <c r="Y73" s="9"/>
-      <c r="AA73" s="5"/>
+      <c r="AA73" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB73" s="31"/>
       <c r="AC73" s="32"/>
       <c r="AD73" s="4"/>
@@ -9050,7 +9204,7 @@
       <c r="AJ73" s="27"/>
       <c r="AK73" s="27"/>
     </row>
-    <row r="74" spans="1:37" ht="41.25" customHeight="1">
+    <row r="74" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>673</v>
       </c>
@@ -9078,7 +9232,9 @@
       <c r="W74" s="26"/>
       <c r="X74" s="9"/>
       <c r="Y74" s="9"/>
-      <c r="AA74" s="5"/>
+      <c r="AA74" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB74" s="31"/>
       <c r="AC74" s="32"/>
       <c r="AD74" s="4"/>
@@ -9090,7 +9246,7 @@
       <c r="AJ74" s="27"/>
       <c r="AK74" s="27"/>
     </row>
-    <row r="75" spans="1:37" ht="41.25" customHeight="1">
+    <row r="75" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>676</v>
       </c>
@@ -9118,7 +9274,9 @@
       <c r="W75" s="26"/>
       <c r="X75" s="9"/>
       <c r="Y75" s="9"/>
-      <c r="AA75" s="5"/>
+      <c r="AA75" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB75" s="31"/>
       <c r="AC75" s="32"/>
       <c r="AD75" s="4"/>
@@ -9130,7 +9288,7 @@
       <c r="AJ75" s="27"/>
       <c r="AK75" s="27"/>
     </row>
-    <row r="76" spans="1:37" ht="41.25" customHeight="1">
+    <row r="76" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>679</v>
       </c>
@@ -9158,7 +9316,9 @@
       <c r="W76" s="26"/>
       <c r="X76" s="9"/>
       <c r="Y76" s="9"/>
-      <c r="AA76" s="5"/>
+      <c r="AA76" s="35">
+        <v>17600</v>
+      </c>
       <c r="AB76" s="31"/>
       <c r="AC76" s="32"/>
       <c r="AD76" s="4"/>
@@ -9170,7 +9330,7 @@
       <c r="AJ76" s="27"/>
       <c r="AK76" s="27"/>
     </row>
-    <row r="77" spans="1:37" ht="41.25" customHeight="1">
+    <row r="77" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>682</v>
       </c>
@@ -9198,7 +9358,9 @@
       <c r="W77" s="26"/>
       <c r="X77" s="9"/>
       <c r="Y77" s="9"/>
-      <c r="AA77" s="5"/>
+      <c r="AA77" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB77" s="31"/>
       <c r="AC77" s="32"/>
       <c r="AD77" s="4"/>
@@ -9210,7 +9372,7 @@
       <c r="AJ77" s="27"/>
       <c r="AK77" s="27"/>
     </row>
-    <row r="78" spans="1:37" ht="41.25" customHeight="1">
+    <row r="78" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>685</v>
       </c>
@@ -9238,7 +9400,9 @@
       <c r="W78" s="26"/>
       <c r="X78" s="9"/>
       <c r="Y78" s="9"/>
-      <c r="AA78" s="5"/>
+      <c r="AA78" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB78" s="31"/>
       <c r="AC78" s="32"/>
       <c r="AD78" s="4"/>
@@ -9250,7 +9414,7 @@
       <c r="AJ78" s="27"/>
       <c r="AK78" s="27"/>
     </row>
-    <row r="79" spans="1:37" ht="41.25" customHeight="1">
+    <row r="79" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>688</v>
       </c>
@@ -9278,7 +9442,9 @@
       <c r="W79" s="26"/>
       <c r="X79" s="9"/>
       <c r="Y79" s="9"/>
-      <c r="AA79" s="5"/>
+      <c r="AA79" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB79" s="31"/>
       <c r="AC79" s="32"/>
       <c r="AD79" s="4"/>
@@ -9290,7 +9456,7 @@
       <c r="AJ79" s="27"/>
       <c r="AK79" s="27"/>
     </row>
-    <row r="80" spans="1:37" ht="41.25" customHeight="1">
+    <row r="80" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>691</v>
       </c>
@@ -9318,7 +9484,9 @@
       <c r="W80" s="26"/>
       <c r="X80" s="9"/>
       <c r="Y80" s="9"/>
-      <c r="AA80" s="5"/>
+      <c r="AA80" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB80" s="31"/>
       <c r="AC80" s="32"/>
       <c r="AD80" s="4"/>
@@ -9330,7 +9498,7 @@
       <c r="AJ80" s="27"/>
       <c r="AK80" s="27"/>
     </row>
-    <row r="81" spans="1:37" ht="41.25" customHeight="1">
+    <row r="81" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>694</v>
       </c>
@@ -9358,7 +9526,9 @@
       <c r="W81" s="26"/>
       <c r="X81" s="9"/>
       <c r="Y81" s="9"/>
-      <c r="AA81" s="5"/>
+      <c r="AA81" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB81" s="31"/>
       <c r="AC81" s="32"/>
       <c r="AD81" s="4"/>
@@ -9370,7 +9540,7 @@
       <c r="AJ81" s="27"/>
       <c r="AK81" s="27"/>
     </row>
-    <row r="82" spans="1:37" ht="41.25" customHeight="1">
+    <row r="82" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>697</v>
       </c>
@@ -9398,7 +9568,9 @@
       <c r="W82" s="26"/>
       <c r="X82" s="9"/>
       <c r="Y82" s="9"/>
-      <c r="AA82" s="5"/>
+      <c r="AA82" s="5" t="s">
+        <v>1108</v>
+      </c>
       <c r="AB82" s="31"/>
       <c r="AC82" s="32"/>
       <c r="AD82" s="4"/>
@@ -9410,7 +9582,7 @@
       <c r="AJ82" s="27"/>
       <c r="AK82" s="27"/>
     </row>
-    <row r="83" spans="1:37" ht="41.25" customHeight="1">
+    <row r="83" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>700</v>
       </c>
@@ -9438,7 +9610,9 @@
       <c r="W83" s="26"/>
       <c r="X83" s="9"/>
       <c r="Y83" s="9"/>
-      <c r="AA83" s="5"/>
+      <c r="AA83" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB83" s="31"/>
       <c r="AC83" s="32"/>
       <c r="AD83" s="4"/>
@@ -9450,7 +9624,7 @@
       <c r="AJ83" s="27"/>
       <c r="AK83" s="27"/>
     </row>
-    <row r="84" spans="1:37" ht="41.25" customHeight="1">
+    <row r="84" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>703</v>
       </c>
@@ -9478,7 +9652,9 @@
       <c r="W84" s="26"/>
       <c r="X84" s="9"/>
       <c r="Y84" s="9"/>
-      <c r="AA84" s="5"/>
+      <c r="AA84" s="35">
+        <v>9400</v>
+      </c>
       <c r="AB84" s="31"/>
       <c r="AC84" s="32"/>
       <c r="AD84" s="4"/>
@@ -9490,7 +9666,7 @@
       <c r="AJ84" s="27"/>
       <c r="AK84" s="27"/>
     </row>
-    <row r="85" spans="1:37" ht="41.25" customHeight="1">
+    <row r="85" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>706</v>
       </c>
@@ -9518,7 +9694,9 @@
       <c r="W85" s="26"/>
       <c r="X85" s="9"/>
       <c r="Y85" s="9"/>
-      <c r="AA85" s="5"/>
+      <c r="AA85" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB85" s="31"/>
       <c r="AC85" s="32"/>
       <c r="AD85" s="4"/>
@@ -9530,7 +9708,7 @@
       <c r="AJ85" s="27"/>
       <c r="AK85" s="27"/>
     </row>
-    <row r="86" spans="1:37" ht="41.25" customHeight="1">
+    <row r="86" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>709</v>
       </c>
@@ -9558,7 +9736,9 @@
       <c r="W86" s="26"/>
       <c r="X86" s="9"/>
       <c r="Y86" s="9"/>
-      <c r="AA86" s="5"/>
+      <c r="AA86" s="5" t="s">
+        <v>1109</v>
+      </c>
       <c r="AB86" s="31"/>
       <c r="AC86" s="32"/>
       <c r="AD86" s="4"/>
@@ -9570,7 +9750,7 @@
       <c r="AJ86" s="27"/>
       <c r="AK86" s="27"/>
     </row>
-    <row r="87" spans="1:37" ht="41.25" customHeight="1">
+    <row r="87" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>712</v>
       </c>
@@ -9598,7 +9778,9 @@
       <c r="W87" s="26"/>
       <c r="X87" s="9"/>
       <c r="Y87" s="9"/>
-      <c r="AA87" s="5"/>
+      <c r="AA87" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB87" s="31"/>
       <c r="AC87" s="32"/>
       <c r="AD87" s="4"/>
@@ -9610,7 +9792,7 @@
       <c r="AJ87" s="27"/>
       <c r="AK87" s="27"/>
     </row>
-    <row r="88" spans="1:37" ht="41.25" customHeight="1">
+    <row r="88" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>715</v>
       </c>
@@ -9638,7 +9820,9 @@
       <c r="W88" s="26"/>
       <c r="X88" s="9"/>
       <c r="Y88" s="9"/>
-      <c r="AA88" s="5"/>
+      <c r="AA88" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB88" s="31"/>
       <c r="AC88" s="32"/>
       <c r="AD88" s="4"/>
@@ -9650,7 +9834,7 @@
       <c r="AJ88" s="27"/>
       <c r="AK88" s="27"/>
     </row>
-    <row r="89" spans="1:37" ht="41.25" customHeight="1">
+    <row r="89" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>718</v>
       </c>
@@ -9678,7 +9862,9 @@
       <c r="W89" s="26"/>
       <c r="X89" s="9"/>
       <c r="Y89" s="9"/>
-      <c r="AA89" s="5"/>
+      <c r="AA89" s="5" t="s">
+        <v>1110</v>
+      </c>
       <c r="AB89" s="31"/>
       <c r="AC89" s="32"/>
       <c r="AD89" s="4"/>
@@ -9690,7 +9876,7 @@
       <c r="AJ89" s="27"/>
       <c r="AK89" s="27"/>
     </row>
-    <row r="90" spans="1:37" ht="41.25" customHeight="1">
+    <row r="90" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>721</v>
       </c>
@@ -9718,7 +9904,9 @@
       <c r="W90" s="26"/>
       <c r="X90" s="9"/>
       <c r="Y90" s="9"/>
-      <c r="AA90" s="5"/>
+      <c r="AA90" s="35">
+        <v>14700</v>
+      </c>
       <c r="AB90" s="31"/>
       <c r="AC90" s="32"/>
       <c r="AD90" s="4"/>
@@ -9730,7 +9918,7 @@
       <c r="AJ90" s="27"/>
       <c r="AK90" s="27"/>
     </row>
-    <row r="91" spans="1:37" ht="41.25" customHeight="1">
+    <row r="91" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>724</v>
       </c>
@@ -9758,7 +9946,9 @@
       <c r="W91" s="26"/>
       <c r="X91" s="9"/>
       <c r="Y91" s="9"/>
-      <c r="AA91" s="5"/>
+      <c r="AA91" s="35">
+        <v>24700</v>
+      </c>
       <c r="AB91" s="31"/>
       <c r="AC91" s="32"/>
       <c r="AD91" s="4"/>
@@ -9770,7 +9960,7 @@
       <c r="AJ91" s="27"/>
       <c r="AK91" s="27"/>
     </row>
-    <row r="92" spans="1:37" ht="41.25" customHeight="1">
+    <row r="92" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>726</v>
       </c>
@@ -9798,7 +9988,9 @@
       <c r="W92" s="26"/>
       <c r="X92" s="9"/>
       <c r="Y92" s="9"/>
-      <c r="AA92" s="5"/>
+      <c r="AA92" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB92" s="31"/>
       <c r="AC92" s="32"/>
       <c r="AD92" s="4"/>
@@ -9810,7 +10002,7 @@
       <c r="AJ92" s="27"/>
       <c r="AK92" s="27"/>
     </row>
-    <row r="93" spans="1:37" ht="41.25" customHeight="1">
+    <row r="93" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>729</v>
       </c>
@@ -9838,7 +10030,9 @@
       <c r="W93" s="26"/>
       <c r="X93" s="9"/>
       <c r="Y93" s="9"/>
-      <c r="AA93" s="5"/>
+      <c r="AA93" s="35">
+        <v>11300</v>
+      </c>
       <c r="AB93" s="31"/>
       <c r="AC93" s="32"/>
       <c r="AD93" s="4"/>
@@ -9850,7 +10044,7 @@
       <c r="AJ93" s="27"/>
       <c r="AK93" s="27"/>
     </row>
-    <row r="94" spans="1:37" ht="41.25" customHeight="1">
+    <row r="94" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>732</v>
       </c>
@@ -9895,7 +10089,9 @@
       <c r="W94" s="26"/>
       <c r="X94" s="9"/>
       <c r="Y94" s="9"/>
-      <c r="AA94" s="5"/>
+      <c r="AA94" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB94" s="31"/>
       <c r="AC94" s="32"/>
       <c r="AD94" s="4"/>
@@ -9907,7 +10103,7 @@
       <c r="AJ94" s="27"/>
       <c r="AK94" s="27"/>
     </row>
-    <row r="95" spans="1:37" ht="41.25" customHeight="1">
+    <row r="95" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>739</v>
       </c>
@@ -9940,7 +10136,9 @@
       <c r="W95" s="26"/>
       <c r="X95" s="9"/>
       <c r="Y95" s="9"/>
-      <c r="AA95" s="5"/>
+      <c r="AA95" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="AB95" s="31"/>
       <c r="AC95" s="32"/>
       <c r="AD95" s="4"/>
@@ -9952,7 +10150,7 @@
       <c r="AJ95" s="27"/>
       <c r="AK95" s="27"/>
     </row>
-    <row r="96" spans="1:37" ht="41.25" customHeight="1">
+    <row r="96" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>745</v>
       </c>
@@ -9987,7 +10185,9 @@
       <c r="W96" s="26"/>
       <c r="X96" s="9"/>
       <c r="Y96" s="9"/>
-      <c r="AA96" s="5"/>
+      <c r="AA96" s="5" t="s">
+        <v>1111</v>
+      </c>
       <c r="AB96" s="31"/>
       <c r="AC96" s="32"/>
       <c r="AD96" s="4"/>
@@ -9999,7 +10199,7 @@
       <c r="AJ96" s="27"/>
       <c r="AK96" s="27"/>
     </row>
-    <row r="97" spans="1:37" ht="41.25" customHeight="1">
+    <row r="97" spans="1:37" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>752</v>
       </c>
@@ -10034,7 +10234,9 @@
       <c r="W97" s="26"/>
       <c r="X97" s="9"/>
       <c r="Y97" s="9"/>
-      <c r="AA97" s="5"/>
+      <c r="AA97" s="35">
+        <v>4800</v>
+      </c>
       <c r="AB97" s="31"/>
       <c r="AC97" s="32"/>
       <c r="AD97" s="4"/>
@@ -10046,9 +10248,17 @@
       <c r="AJ97" s="27"/>
       <c r="AK97" s="27"/>
     </row>
-    <row r="98" spans="1:37" ht="12">
-      <c r="B98" s="9"/>
+    <row r="98" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>1087</v>
+      </c>
       <c r="C98" s="9"/>
+      <c r="F98" t="s">
+        <v>1097</v>
+      </c>
       <c r="G98" s="9"/>
       <c r="H98" s="28"/>
       <c r="K98" s="9"/>
@@ -10076,9 +10286,17 @@
       <c r="AJ98" s="27"/>
       <c r="AK98" s="27"/>
     </row>
-    <row r="99" spans="1:37" ht="12">
-      <c r="B99" s="9"/>
+    <row r="99" spans="1:37" ht="102" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>1088</v>
+      </c>
       <c r="C99" s="9"/>
+      <c r="F99" s="34" t="s">
+        <v>1098</v>
+      </c>
       <c r="G99" s="9"/>
       <c r="H99" s="28"/>
       <c r="J99" s="9"/>
@@ -10107,9 +10325,17 @@
       <c r="AJ99" s="27"/>
       <c r="AK99" s="27"/>
     </row>
-    <row r="100" spans="1:37" ht="12">
-      <c r="B100" s="9"/>
+    <row r="100" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>1089</v>
+      </c>
       <c r="C100" s="9"/>
+      <c r="F100" t="s">
+        <v>1099</v>
+      </c>
       <c r="G100" s="9"/>
       <c r="H100" s="28"/>
       <c r="J100" s="9"/>
@@ -10138,9 +10364,17 @@
       <c r="AJ100" s="27"/>
       <c r="AK100" s="27"/>
     </row>
-    <row r="101" spans="1:37" ht="12">
-      <c r="B101" s="9"/>
+    <row r="101" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>1090</v>
+      </c>
       <c r="C101" s="9"/>
+      <c r="F101" t="s">
+        <v>1104</v>
+      </c>
       <c r="G101" s="9"/>
       <c r="H101" s="28"/>
       <c r="J101" s="9"/>
@@ -10169,9 +10403,17 @@
       <c r="AJ101" s="27"/>
       <c r="AK101" s="27"/>
     </row>
-    <row r="102" spans="1:37" ht="12">
-      <c r="B102" s="9"/>
+    <row r="102" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>1091</v>
+      </c>
       <c r="C102" s="9"/>
+      <c r="F102" t="s">
+        <v>1105</v>
+      </c>
       <c r="G102" s="9"/>
       <c r="H102" s="28"/>
       <c r="J102" s="9"/>
@@ -10200,9 +10442,17 @@
       <c r="AJ102" s="27"/>
       <c r="AK102" s="27"/>
     </row>
-    <row r="103" spans="1:37" ht="12">
-      <c r="B103" s="9"/>
+    <row r="103" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>1092</v>
+      </c>
       <c r="C103" s="9"/>
+      <c r="F103" t="s">
+        <v>1106</v>
+      </c>
       <c r="G103" s="9"/>
       <c r="H103" s="28"/>
       <c r="J103" s="9"/>
@@ -10231,9 +10481,17 @@
       <c r="AJ103" s="27"/>
       <c r="AK103" s="27"/>
     </row>
-    <row r="104" spans="1:37" ht="12">
-      <c r="B104" s="9"/>
+    <row r="104" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>1093</v>
+      </c>
       <c r="C104" s="9"/>
+      <c r="F104" t="s">
+        <v>1100</v>
+      </c>
       <c r="G104" s="9"/>
       <c r="H104" s="28"/>
       <c r="J104" s="9"/>
@@ -10262,9 +10520,17 @@
       <c r="AJ104" s="27"/>
       <c r="AK104" s="27"/>
     </row>
-    <row r="105" spans="1:37" ht="12">
-      <c r="B105" s="9"/>
+    <row r="105" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>1094</v>
+      </c>
       <c r="C105" s="9"/>
+      <c r="F105" t="s">
+        <v>1101</v>
+      </c>
       <c r="G105" s="9"/>
       <c r="H105" s="28"/>
       <c r="J105" s="9"/>
@@ -10293,9 +10559,17 @@
       <c r="AJ105" s="27"/>
       <c r="AK105" s="27"/>
     </row>
-    <row r="106" spans="1:37" ht="12">
-      <c r="B106" s="9"/>
+    <row r="106" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>1095</v>
+      </c>
       <c r="C106" s="9"/>
+      <c r="F106" t="s">
+        <v>1102</v>
+      </c>
       <c r="G106" s="9"/>
       <c r="H106" s="28"/>
       <c r="J106" s="9"/>
@@ -10324,9 +10598,17 @@
       <c r="AJ106" s="27"/>
       <c r="AK106" s="27"/>
     </row>
-    <row r="107" spans="1:37" ht="12">
-      <c r="B107" s="9"/>
+    <row r="107" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>1096</v>
+      </c>
       <c r="C107" s="9"/>
+      <c r="F107" t="s">
+        <v>1103</v>
+      </c>
       <c r="G107" s="9"/>
       <c r="H107" s="28"/>
       <c r="J107" s="9"/>
@@ -10355,7 +10637,7 @@
       <c r="AJ107" s="27"/>
       <c r="AK107" s="27"/>
     </row>
-    <row r="108" spans="1:37" ht="12">
+    <row r="108" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B108" s="9"/>
       <c r="C108" s="9"/>
       <c r="G108" s="9"/>
@@ -10386,7 +10668,7 @@
       <c r="AJ108" s="27"/>
       <c r="AK108" s="27"/>
     </row>
-    <row r="109" spans="1:37" ht="12">
+    <row r="109" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B109" s="9"/>
       <c r="C109" s="9"/>
       <c r="G109" s="9"/>
@@ -10417,7 +10699,7 @@
       <c r="AJ109" s="27"/>
       <c r="AK109" s="27"/>
     </row>
-    <row r="110" spans="1:37" ht="12">
+    <row r="110" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B110" s="9"/>
       <c r="C110" s="9"/>
       <c r="G110" s="9"/>
@@ -10448,7 +10730,7 @@
       <c r="AJ110" s="27"/>
       <c r="AK110" s="27"/>
     </row>
-    <row r="111" spans="1:37" ht="12">
+    <row r="111" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
       <c r="G111" s="9"/>
@@ -10479,7 +10761,7 @@
       <c r="AJ111" s="27"/>
       <c r="AK111" s="27"/>
     </row>
-    <row r="112" spans="1:37" ht="12">
+    <row r="112" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B112" s="9"/>
       <c r="C112" s="9"/>
       <c r="G112" s="9"/>
@@ -10510,7 +10792,7 @@
       <c r="AJ112" s="27"/>
       <c r="AK112" s="27"/>
     </row>
-    <row r="113" spans="2:37" ht="12">
+    <row r="113" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
       <c r="G113" s="9"/>
@@ -10541,7 +10823,7 @@
       <c r="AJ113" s="27"/>
       <c r="AK113" s="27"/>
     </row>
-    <row r="114" spans="2:37" ht="12">
+    <row r="114" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B114" s="9"/>
       <c r="C114" s="9"/>
       <c r="G114" s="9"/>
@@ -10572,7 +10854,7 @@
       <c r="AJ114" s="27"/>
       <c r="AK114" s="27"/>
     </row>
-    <row r="115" spans="2:37" ht="12">
+    <row r="115" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B115" s="9"/>
       <c r="C115" s="9"/>
       <c r="G115" s="9"/>
@@ -10603,7 +10885,7 @@
       <c r="AJ115" s="27"/>
       <c r="AK115" s="27"/>
     </row>
-    <row r="116" spans="2:37" ht="12">
+    <row r="116" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B116" s="9"/>
       <c r="C116" s="9"/>
       <c r="G116" s="9"/>
@@ -10634,7 +10916,7 @@
       <c r="AJ116" s="27"/>
       <c r="AK116" s="27"/>
     </row>
-    <row r="117" spans="2:37" ht="12">
+    <row r="117" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B117" s="9"/>
       <c r="C117" s="9"/>
       <c r="G117" s="9"/>
@@ -10665,7 +10947,7 @@
       <c r="AJ117" s="27"/>
       <c r="AK117" s="27"/>
     </row>
-    <row r="118" spans="2:37" ht="12">
+    <row r="118" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B118" s="9"/>
       <c r="C118" s="9"/>
       <c r="G118" s="9"/>
@@ -10697,6 +10979,9 @@
       <c r="AK118" s="27"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F99" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -10717,12 +11002,12 @@
       <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="41.25" customHeight="1">
+    <row r="1" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="str">
         <f>All!A1</f>
         <v>Compound Identifier</v>
@@ -10880,7 +11165,7 @@
         <v>In vivo mouse P. Berghei oral 50 mg/kg</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="41.25" customHeight="1">
+    <row r="2" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="str">
         <f>All!A3</f>
         <v>OSM-S-2</v>
@@ -11035,7 +11320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="41.25" customHeight="1">
+    <row r="3" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="str">
         <f>All!A4</f>
         <v>OSM-S-3</v>
@@ -11190,7 +11475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="41.25" customHeight="1">
+    <row r="4" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="str">
         <f>All!A5</f>
         <v>OSM-S-4</v>
@@ -11345,7 +11630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="41.25" customHeight="1">
+    <row r="5" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="str">
         <f>All!A6</f>
         <v>OSM-S-5</v>
@@ -11500,7 +11785,7 @@
         <v>neg</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="41.25" customHeight="1">
+    <row r="6" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="str">
         <f>All!A7</f>
         <v>OSM-S-6</v>
@@ -11655,7 +11940,7 @@
         <v>neg</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="41.25" customHeight="1">
+    <row r="7" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="str">
         <f>All!A10</f>
         <v>OSM-S-9</v>
@@ -11810,7 +12095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="41.25" customHeight="1">
+    <row r="8" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="str">
         <f>All!A11</f>
         <v>OSM-S-10</v>
@@ -11965,7 +12250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:39" ht="41.25" customHeight="1">
+    <row r="9" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="str">
         <f>All!A12</f>
         <v>OSM-S-11</v>
@@ -12120,7 +12405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="41.25" customHeight="1">
+    <row r="10" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="str">
         <f>All!A14</f>
         <v>OSM-S-13</v>
@@ -12275,7 +12560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="41.25" customHeight="1">
+    <row r="11" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="str">
         <f>All!A15</f>
         <v>OSM-S-14</v>
@@ -12430,7 +12715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="41.25" customHeight="1">
+    <row r="12" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="str">
         <f>All!A20</f>
         <v>OSM-S-19</v>
@@ -12585,7 +12870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="41.25" customHeight="1">
+    <row r="13" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="str">
         <f>All!A22</f>
         <v>OSM-S-21</v>
@@ -12740,7 +13025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="41.25" customHeight="1">
+    <row r="14" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="str">
         <f>All!A29</f>
         <v>OSM-S-28</v>
@@ -12895,7 +13180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="41.25" customHeight="1">
+    <row r="15" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="str">
         <f>All!A30</f>
         <v>OSM-S-29</v>
@@ -13050,7 +13335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:39" ht="41.25" customHeight="1">
+    <row r="16" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="str">
         <f>All!A31</f>
         <v>OSM-S-30</v>
@@ -13205,7 +13490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:39" ht="41.25" customHeight="1">
+    <row r="17" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="str">
         <f>All!A32</f>
         <v>OSM-S-31</v>
@@ -13360,7 +13645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="41.25" customHeight="1">
+    <row r="18" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="str">
         <f>All!A33</f>
         <v>OSM-S-32</v>
@@ -13515,7 +13800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:39" ht="41.25" customHeight="1">
+    <row r="19" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="str">
         <f>All!A37</f>
         <v>OSM-S-36</v>
@@ -13670,7 +13955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:39" ht="41.25" customHeight="1">
+    <row r="20" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="str">
         <f>All!A39</f>
         <v>OSM-S-38</v>
@@ -13825,7 +14110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:39" ht="41.25" customHeight="1">
+    <row r="21" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="str">
         <f>All!A40</f>
         <v>OSM-S-39</v>
@@ -13980,7 +14265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:39" ht="41.25" customHeight="1">
+    <row r="22" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="str">
         <f>All!A36</f>
         <v>OSM-S-35</v>
@@ -14135,7 +14420,7 @@
         <v>neg</v>
       </c>
     </row>
-    <row r="23" spans="1:39" ht="41.25" customHeight="1">
+    <row r="23" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="str">
         <f>All!A43</f>
         <v>OSM-S-42</v>
@@ -14290,7 +14575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:39" ht="41.25" customHeight="1">
+    <row r="24" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="str">
         <f>All!A44</f>
         <v>OSM-S-43</v>
@@ -14445,7 +14730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:39" ht="41.25" customHeight="1">
+    <row r="25" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="str">
         <f>All!A38</f>
         <v>OSM-S-37</v>
@@ -14600,7 +14885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:39" ht="41.25" customHeight="1">
+    <row r="26" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="str">
         <f>All!A46</f>
         <v>OSM-S-45</v>
@@ -14755,7 +15040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:39" ht="41.25" customHeight="1">
+    <row r="27" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="str">
         <f>All!A49</f>
         <v>OSM-S-48</v>
@@ -14910,7 +15195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="41.25" customHeight="1">
+    <row r="28" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="str">
         <f>All!A50</f>
         <v>OSM-S-49</v>
@@ -15065,7 +15350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:39" ht="41.25" customHeight="1">
+    <row r="29" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="str">
         <f>All!A51</f>
         <v>OSM-S-50</v>
@@ -15220,7 +15505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:39" ht="41.25" customHeight="1">
+    <row r="30" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="str">
         <f>All!A52</f>
         <v>OSM-S-51</v>
@@ -15375,7 +15660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:39" ht="41.25" customHeight="1">
+    <row r="31" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="str">
         <f>All!A53</f>
         <v>OSM-S-52</v>
@@ -15530,7 +15815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="41.25" customHeight="1">
+    <row r="32" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="str">
         <f>All!A55</f>
         <v>OSM-S-54</v>
@@ -15685,7 +15970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:39" ht="41.25" customHeight="1">
+    <row r="33" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="str">
         <f>All!A56</f>
         <v>OSM-S-55</v>
@@ -15840,7 +16125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:39" ht="41.25" customHeight="1">
+    <row r="34" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="str">
         <f>All!A57</f>
         <v>OSM-S-56</v>
@@ -15947,7 +16232,7 @@
       </c>
       <c r="AA34" s="11">
         <f>All!AA57</f>
-        <v>0</v>
+        <v>333</v>
       </c>
       <c r="AB34" s="30">
         <f>All!AB57</f>
@@ -15998,7 +16283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:39" ht="41.25" customHeight="1">
+    <row r="35" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="str">
         <f>All!A58</f>
         <v>OSM-S-57</v>
@@ -16103,9 +16388,9 @@
         <f>All!Z58</f>
         <v>0.81</v>
       </c>
-      <c r="AA35" s="11">
+      <c r="AA35" s="11" t="str">
         <f>All!AA58</f>
-        <v>0</v>
+        <v>&gt;100000</v>
       </c>
       <c r="AB35" s="30">
         <f>All!AB58</f>
@@ -16156,7 +16441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:39" ht="41.25" customHeight="1">
+    <row r="36" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="str">
         <f>All!A59</f>
         <v>OSM-S-58</v>
@@ -16261,9 +16546,9 @@
         <f>All!Z59</f>
         <v>0</v>
       </c>
-      <c r="AA36" s="11">
+      <c r="AA36" s="11" t="str">
         <f>All!AA59</f>
-        <v>0</v>
+        <v>&gt;100000</v>
       </c>
       <c r="AB36" s="30">
         <f>All!AB59</f>
@@ -16314,7 +16599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:39" ht="41.25" customHeight="1">
+    <row r="37" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="str">
         <f>All!A60</f>
         <v>OSM-S-59</v>
@@ -16419,9 +16704,9 @@
         <f>All!Z60</f>
         <v>0</v>
       </c>
-      <c r="AA37" s="11">
+      <c r="AA37" s="11" t="str">
         <f>All!AA60</f>
-        <v>0</v>
+        <v>&gt;100000</v>
       </c>
       <c r="AB37" s="30">
         <f>All!AB60</f>
@@ -16472,7 +16757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:39" ht="41.25" customHeight="1">
+    <row r="38" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="str">
         <f>All!A61</f>
         <v>OSM-S-60</v>
@@ -16516,7 +16801,7 @@
       <c r="AL38" s="3"/>
       <c r="AM38" s="3"/>
     </row>
-    <row r="39" spans="1:39" ht="41.25" customHeight="1">
+    <row r="39" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="str">
         <f>All!A62</f>
         <v>OSM-S-61</v>
@@ -16560,7 +16845,7 @@
       <c r="AL39" s="3"/>
       <c r="AM39" s="3"/>
     </row>
-    <row r="40" spans="1:39" ht="41.25" customHeight="1">
+    <row r="40" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="str">
         <f>All!A63</f>
         <v>OSM-S-62</v>
@@ -16604,7 +16889,7 @@
       <c r="AL40" s="3"/>
       <c r="AM40" s="3"/>
     </row>
-    <row r="41" spans="1:39" ht="41.25" customHeight="1">
+    <row r="41" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="str">
         <f>All!A64</f>
         <v>OSM-S-63</v>
@@ -16648,7 +16933,7 @@
       <c r="AL41" s="3"/>
       <c r="AM41" s="3"/>
     </row>
-    <row r="42" spans="1:39" ht="41.25" customHeight="1">
+    <row r="42" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -16689,7 +16974,7 @@
       <c r="AL42" s="3"/>
       <c r="AM42" s="3"/>
     </row>
-    <row r="43" spans="1:39" ht="41.25" customHeight="1">
+    <row r="43" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -16730,7 +17015,7 @@
       <c r="AL43" s="3"/>
       <c r="AM43" s="3"/>
     </row>
-    <row r="44" spans="1:39" ht="41.25" customHeight="1">
+    <row r="44" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -16771,7 +17056,7 @@
       <c r="AL44" s="3"/>
       <c r="AM44" s="3"/>
     </row>
-    <row r="45" spans="1:39" ht="41.25" customHeight="1">
+    <row r="45" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -16812,7 +17097,7 @@
       <c r="AL45" s="3"/>
       <c r="AM45" s="3"/>
     </row>
-    <row r="46" spans="1:39" ht="41.25" customHeight="1">
+    <row r="46" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -16853,7 +17138,7 @@
       <c r="AL46" s="3"/>
       <c r="AM46" s="3"/>
     </row>
-    <row r="47" spans="1:39" ht="41.25" customHeight="1">
+    <row r="47" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -16894,7 +17179,7 @@
       <c r="AL47" s="3"/>
       <c r="AM47" s="3"/>
     </row>
-    <row r="48" spans="1:39" ht="41.25" customHeight="1">
+    <row r="48" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -16935,7 +17220,7 @@
       <c r="AL48" s="3"/>
       <c r="AM48" s="3"/>
     </row>
-    <row r="49" spans="1:39" ht="41.25" customHeight="1">
+    <row r="49" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -16976,7 +17261,7 @@
       <c r="AL49" s="3"/>
       <c r="AM49" s="3"/>
     </row>
-    <row r="50" spans="1:39" ht="41.25" customHeight="1">
+    <row r="50" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -17017,7 +17302,7 @@
       <c r="AL50" s="3"/>
       <c r="AM50" s="3"/>
     </row>
-    <row r="51" spans="1:39" ht="41.25" customHeight="1">
+    <row r="51" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -17058,7 +17343,7 @@
       <c r="AL51" s="3"/>
       <c r="AM51" s="3"/>
     </row>
-    <row r="52" spans="1:39" ht="41.25" customHeight="1">
+    <row r="52" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -17099,7 +17384,7 @@
       <c r="AL52" s="3"/>
       <c r="AM52" s="3"/>
     </row>
-    <row r="53" spans="1:39" ht="41.25" customHeight="1">
+    <row r="53" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -17140,7 +17425,7 @@
       <c r="AL53" s="3"/>
       <c r="AM53" s="3"/>
     </row>
-    <row r="54" spans="1:39" ht="41.25" customHeight="1">
+    <row r="54" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -17181,7 +17466,7 @@
       <c r="AL54" s="3"/>
       <c r="AM54" s="3"/>
     </row>
-    <row r="55" spans="1:39" ht="41.25" customHeight="1">
+    <row r="55" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -17222,7 +17507,7 @@
       <c r="AL55" s="3"/>
       <c r="AM55" s="3"/>
     </row>
-    <row r="56" spans="1:39" ht="41.25" customHeight="1">
+    <row r="56" spans="1:39" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -17263,7 +17548,7 @@
       <c r="AL56" s="3"/>
       <c r="AM56" s="3"/>
     </row>
-    <row r="57" spans="1:39" ht="12">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -17304,7 +17589,7 @@
       <c r="AL57" s="3"/>
       <c r="AM57" s="3"/>
     </row>
-    <row r="58" spans="1:39" ht="12">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -17345,7 +17630,7 @@
       <c r="AL58" s="3"/>
       <c r="AM58" s="3"/>
     </row>
-    <row r="59" spans="1:39" ht="12">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -17386,7 +17671,7 @@
       <c r="AL59" s="3"/>
       <c r="AM59" s="3"/>
     </row>
-    <row r="60" spans="1:39" ht="12">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -17427,7 +17712,7 @@
       <c r="AL60" s="3"/>
       <c r="AM60" s="3"/>
     </row>
-    <row r="61" spans="1:39" ht="12">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -17468,7 +17753,7 @@
       <c r="AL61" s="3"/>
       <c r="AM61" s="3"/>
     </row>
-    <row r="62" spans="1:39" ht="12">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -17509,7 +17794,7 @@
       <c r="AL62" s="3"/>
       <c r="AM62" s="3"/>
     </row>
-    <row r="63" spans="1:39" ht="12">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -17550,7 +17835,7 @@
       <c r="AL63" s="3"/>
       <c r="AM63" s="3"/>
     </row>
-    <row r="64" spans="1:39" ht="12">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -17591,7 +17876,7 @@
       <c r="AL64" s="3"/>
       <c r="AM64" s="3"/>
     </row>
-    <row r="65" spans="1:39" ht="12">
+    <row r="65" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -17632,7 +17917,7 @@
       <c r="AL65" s="3"/>
       <c r="AM65" s="3"/>
     </row>
-    <row r="66" spans="1:39" ht="12">
+    <row r="66" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -17673,7 +17958,7 @@
       <c r="AL66" s="3"/>
       <c r="AM66" s="3"/>
     </row>
-    <row r="67" spans="1:39" ht="12">
+    <row r="67" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -17714,7 +17999,7 @@
       <c r="AL67" s="3"/>
       <c r="AM67" s="3"/>
     </row>
-    <row r="68" spans="1:39" ht="12">
+    <row r="68" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -17755,7 +18040,7 @@
       <c r="AL68" s="3"/>
       <c r="AM68" s="3"/>
     </row>
-    <row r="69" spans="1:39" ht="12">
+    <row r="69" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -17796,7 +18081,7 @@
       <c r="AL69" s="3"/>
       <c r="AM69" s="3"/>
     </row>
-    <row r="70" spans="1:39" ht="12">
+    <row r="70" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -17837,7 +18122,7 @@
       <c r="AL70" s="3"/>
       <c r="AM70" s="3"/>
     </row>
-    <row r="71" spans="1:39" ht="12">
+    <row r="71" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -17878,7 +18163,7 @@
       <c r="AL71" s="3"/>
       <c r="AM71" s="3"/>
     </row>
-    <row r="72" spans="1:39" ht="12">
+    <row r="72" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -17919,7 +18204,7 @@
       <c r="AL72" s="3"/>
       <c r="AM72" s="3"/>
     </row>
-    <row r="73" spans="1:39" ht="12">
+    <row r="73" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -17960,7 +18245,7 @@
       <c r="AL73" s="3"/>
       <c r="AM73" s="3"/>
     </row>
-    <row r="74" spans="1:39" ht="12">
+    <row r="74" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -18001,7 +18286,7 @@
       <c r="AL74" s="3"/>
       <c r="AM74" s="3"/>
     </row>
-    <row r="75" spans="1:39" ht="12">
+    <row r="75" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -18042,7 +18327,7 @@
       <c r="AL75" s="3"/>
       <c r="AM75" s="3"/>
     </row>
-    <row r="76" spans="1:39" ht="12">
+    <row r="76" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -18083,7 +18368,7 @@
       <c r="AL76" s="3"/>
       <c r="AM76" s="3"/>
     </row>
-    <row r="77" spans="1:39" ht="12">
+    <row r="77" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -18145,14 +18430,14 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="20" max="20" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="20" max="20" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="14.25" customHeight="1">
+    <row r="1" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="str">
         <f>All!C1</f>
         <v>Name</v>
@@ -18222,7 +18507,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="67.5" customHeight="1">
+    <row r="2" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -18258,7 +18543,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="67.5" customHeight="1">
+    <row r="3" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
       <c r="B3" s="9">
         <v>2</v>
@@ -18296,7 +18581,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="67.5" customHeight="1">
+    <row r="4" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
       <c r="B4" s="9">
         <v>1</v>
@@ -18334,7 +18619,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="67.5" customHeight="1">
+    <row r="5" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -18370,7 +18655,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="67.5" customHeight="1">
+    <row r="6" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -18406,7 +18691,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="67.5" customHeight="1">
+    <row r="7" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -18442,7 +18727,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="67.5" customHeight="1">
+    <row r="8" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -18478,7 +18763,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="67.5" customHeight="1">
+    <row r="9" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -18514,7 +18799,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="67.5" customHeight="1">
+    <row r="10" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -18550,7 +18835,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="67.5" customHeight="1">
+    <row r="11" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -18586,7 +18871,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="67.5" customHeight="1">
+    <row r="12" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -18622,7 +18907,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="67.5" customHeight="1">
+    <row r="13" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -18658,7 +18943,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="67.5" customHeight="1">
+    <row r="14" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -18694,7 +18979,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="67.5" customHeight="1">
+    <row r="15" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -18730,7 +19015,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="67.5" customHeight="1">
+    <row r="16" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -18766,7 +19051,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="67.5" customHeight="1">
+    <row r="17" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -18802,7 +19087,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="67.5" customHeight="1">
+    <row r="18" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -18844,7 +19129,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="67.5" customHeight="1">
+    <row r="19" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -18886,7 +19171,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="67.5" customHeight="1">
+    <row r="20" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -18926,7 +19211,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="67.5" customHeight="1">
+    <row r="21" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -18968,7 +19253,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="67.5" customHeight="1">
+    <row r="22" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -19010,7 +19295,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="67.5" customHeight="1">
+    <row r="23" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -19052,7 +19337,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="67.5" customHeight="1">
+    <row r="24" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -19094,7 +19379,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="67.5" customHeight="1">
+    <row r="25" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -19136,7 +19421,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="67.5" customHeight="1">
+    <row r="26" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" s="9"/>
       <c r="D26" s="9" t="s">
         <v>819</v>
@@ -19170,7 +19455,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="67.5" customHeight="1">
+    <row r="27" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C27" s="9"/>
       <c r="D27" s="9" t="s">
         <v>819</v>
@@ -19204,7 +19489,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="67.5" customHeight="1">
+    <row r="28" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>1</v>
       </c>
@@ -19237,7 +19522,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="67.5" customHeight="1">
+    <row r="29" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C29" s="9"/>
       <c r="D29" t="s">
         <v>898</v>
@@ -19267,7 +19552,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="67.5" customHeight="1">
+    <row r="30" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>1</v>
       </c>
@@ -19300,7 +19585,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="67.5" customHeight="1">
+    <row r="31" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C31" s="9"/>
       <c r="D31" t="s">
         <v>898</v>
@@ -19330,7 +19615,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="67.5" customHeight="1">
+    <row r="32" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C32" s="9"/>
       <c r="D32" t="s">
         <v>898</v>
@@ -19360,7 +19645,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="33" spans="2:20" ht="67.5" customHeight="1">
+    <row r="33" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>1</v>
       </c>
@@ -19393,7 +19678,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="34" spans="2:20" ht="67.5" customHeight="1">
+    <row r="34" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>1</v>
       </c>
@@ -19426,7 +19711,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="35" spans="2:20" ht="67.5" customHeight="1">
+    <row r="35" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C35" s="9"/>
       <c r="D35" t="s">
         <v>919</v>
@@ -19456,7 +19741,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="36" spans="2:20" ht="67.5" customHeight="1">
+    <row r="36" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="9"/>
       <c r="D36" t="s">
         <v>919</v>
@@ -19486,7 +19771,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="37" spans="2:20" ht="67.5" customHeight="1">
+    <row r="37" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37">
         <v>1</v>
       </c>
@@ -19519,7 +19804,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="38" spans="2:20" ht="67.5" customHeight="1">
+    <row r="38" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38">
         <v>1</v>
       </c>
@@ -19552,7 +19837,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="39" spans="2:20" ht="67.5" customHeight="1">
+    <row r="39" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39">
         <v>1</v>
       </c>
@@ -19585,7 +19870,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="40" spans="2:20" ht="67.5" customHeight="1">
+    <row r="40" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="9"/>
       <c r="D40" t="s">
         <v>919</v>
@@ -19615,7 +19900,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="41" spans="2:20" ht="67.5" customHeight="1">
+    <row r="41" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="9"/>
       <c r="D41" t="s">
         <v>919</v>
@@ -19645,7 +19930,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="42" spans="2:20" ht="67.5" customHeight="1">
+    <row r="42" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="9"/>
       <c r="D42" t="s">
         <v>919</v>
@@ -19675,7 +19960,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="43" spans="2:20" ht="67.5" customHeight="1">
+    <row r="43" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>1</v>
       </c>
@@ -19708,7 +19993,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="44" spans="2:20" ht="67.5" customHeight="1">
+    <row r="44" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44">
         <v>1</v>
       </c>
@@ -19741,7 +20026,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="45" spans="2:20" ht="67.5" customHeight="1">
+    <row r="45" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C45" s="9"/>
       <c r="D45" t="s">
         <v>919</v>
@@ -19771,7 +20056,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="46" spans="2:20" ht="67.5" customHeight="1">
+    <row r="46" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C46" s="9"/>
       <c r="D46" t="s">
         <v>919</v>
@@ -19801,7 +20086,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="47" spans="2:20" ht="67.5" customHeight="1">
+    <row r="47" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C47" s="9"/>
       <c r="D47" t="s">
         <v>919</v>
@@ -19831,7 +20116,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="48" spans="2:20" ht="67.5" customHeight="1">
+    <row r="48" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C48" s="9"/>
       <c r="D48" t="s">
         <v>919</v>
@@ -19861,7 +20146,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="49" spans="2:20" ht="67.5" customHeight="1">
+    <row r="49" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49">
         <v>1</v>
       </c>
@@ -19894,7 +20179,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="50" spans="2:20" ht="67.5" customHeight="1">
+    <row r="50" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50">
         <v>1</v>
       </c>
@@ -19927,7 +20212,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="51" spans="2:20" ht="67.5" customHeight="1">
+    <row r="51" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51">
         <v>1</v>
       </c>
@@ -19960,7 +20245,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="52" spans="2:20" ht="67.5" customHeight="1">
+    <row r="52" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C52" s="9"/>
       <c r="D52" t="s">
         <v>919</v>
@@ -19990,7 +20275,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="53" spans="2:20" ht="67.5" customHeight="1">
+    <row r="53" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C53" s="9"/>
       <c r="D53" t="s">
         <v>919</v>
@@ -20020,7 +20305,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="54" spans="2:20" ht="67.5" customHeight="1">
+    <row r="54" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C54" s="9"/>
       <c r="D54" t="s">
         <v>919</v>
@@ -20050,7 +20335,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="55" spans="2:20" ht="67.5" customHeight="1">
+    <row r="55" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C55" s="9"/>
       <c r="D55" t="s">
         <v>919</v>
@@ -20080,7 +20365,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="56" spans="2:20" ht="67.5" customHeight="1">
+    <row r="56" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56">
         <v>1</v>
       </c>
@@ -20113,7 +20398,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="57" spans="2:20" ht="67.5" customHeight="1">
+    <row r="57" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C57" s="9"/>
       <c r="D57" t="s">
         <v>919</v>
@@ -20143,7 +20428,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="58" spans="2:20" ht="67.5" customHeight="1">
+    <row r="58" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58">
         <v>1</v>
       </c>
@@ -20176,7 +20461,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="59" spans="2:20" ht="67.5" customHeight="1">
+    <row r="59" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59">
         <v>1</v>
       </c>
@@ -20209,7 +20494,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="60" spans="2:20" ht="67.5" customHeight="1">
+    <row r="60" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60">
         <v>1</v>
       </c>
@@ -20242,7 +20527,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="61" spans="2:20" ht="67.5" customHeight="1">
+    <row r="61" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C61" s="9"/>
       <c r="D61" t="s">
         <v>919</v>
@@ -20272,7 +20557,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="62" spans="2:20" ht="67.5" customHeight="1">
+    <row r="62" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C62" s="9"/>
       <c r="D62" t="s">
         <v>919</v>
@@ -20302,7 +20587,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="63" spans="2:20" ht="67.5" customHeight="1">
+    <row r="63" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63">
         <v>1</v>
       </c>
@@ -20335,7 +20620,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="64" spans="2:20" ht="67.5" customHeight="1">
+    <row r="64" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C64" s="9"/>
       <c r="D64" t="s">
         <v>919</v>
@@ -20365,7 +20650,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="65" spans="2:20" ht="67.5" customHeight="1">
+    <row r="65" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65">
         <v>1</v>
       </c>
@@ -20398,7 +20683,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="66" spans="2:20" ht="67.5" customHeight="1">
+    <row r="66" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66">
         <v>1</v>
       </c>
@@ -20431,7 +20716,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="67" spans="2:20" ht="67.5" customHeight="1">
+    <row r="67" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C67" s="9"/>
       <c r="D67" t="s">
         <v>919</v>
@@ -20461,7 +20746,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="68" spans="2:20" ht="67.5" customHeight="1">
+    <row r="68" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C68" s="9"/>
       <c r="D68" t="s">
         <v>919</v>
@@ -20491,7 +20776,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="69" spans="2:20" ht="67.5" customHeight="1">
+    <row r="69" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69">
         <v>1</v>
       </c>
@@ -20524,7 +20809,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="70" spans="2:20" ht="67.5" customHeight="1">
+    <row r="70" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70">
         <v>1</v>
       </c>
@@ -20557,7 +20842,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="71" spans="2:20" ht="67.5" customHeight="1">
+    <row r="71" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71">
         <v>1</v>
       </c>
@@ -20590,7 +20875,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="72" spans="2:20" ht="67.5" customHeight="1">
+    <row r="72" spans="2:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72">
         <v>1</v>
       </c>
@@ -20623,7 +20908,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="73" spans="2:20" ht="56.25" customHeight="1">
+    <row r="73" spans="2:20" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C73" s="9" t="s">
         <v>1066</v>
       </c>
@@ -20636,7 +20921,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="74" spans="2:20" ht="56.25" customHeight="1">
+    <row r="74" spans="2:20" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C74" s="9" t="s">
         <v>1067</v>
       </c>
@@ -20646,7 +20931,7 @@
       <c r="L74" s="9"/>
       <c r="Q74" s="10"/>
     </row>
-    <row r="75" spans="2:20" ht="56.25" customHeight="1">
+    <row r="75" spans="2:20" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C75" s="9" t="s">
         <v>1067</v>
       </c>
@@ -20656,175 +20941,175 @@
       <c r="L75" s="9"/>
       <c r="Q75" s="10"/>
     </row>
-    <row r="76" spans="2:20" ht="56.25" customHeight="1">
+    <row r="76" spans="2:20" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G76" s="9"/>
       <c r="H76" s="23"/>
       <c r="I76" s="23"/>
       <c r="L76" s="9"/>
       <c r="Q76" s="10"/>
     </row>
-    <row r="77" spans="2:20" ht="56.25" customHeight="1">
+    <row r="77" spans="2:20" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G77" s="9"/>
       <c r="H77" s="23"/>
       <c r="I77" s="23"/>
       <c r="L77" s="9"/>
       <c r="Q77" s="10"/>
     </row>
-    <row r="78" spans="2:20" ht="56.25" customHeight="1">
+    <row r="78" spans="2:20" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G78" s="9"/>
       <c r="H78" s="23"/>
       <c r="I78" s="23"/>
       <c r="L78" s="9"/>
       <c r="Q78" s="10"/>
     </row>
-    <row r="79" spans="2:20" ht="56.25" customHeight="1">
+    <row r="79" spans="2:20" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G79" s="9"/>
       <c r="H79" s="23"/>
       <c r="I79" s="23"/>
       <c r="L79" s="9"/>
       <c r="Q79" s="10"/>
     </row>
-    <row r="80" spans="2:20" ht="12">
+    <row r="80" spans="2:20" x14ac:dyDescent="0.2">
       <c r="G80" s="9"/>
       <c r="H80" s="23"/>
       <c r="I80" s="23"/>
       <c r="L80" s="9"/>
       <c r="Q80" s="10"/>
     </row>
-    <row r="81" spans="7:17" ht="12">
+    <row r="81" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G81" s="9"/>
       <c r="H81" s="23"/>
       <c r="I81" s="23"/>
       <c r="L81" s="9"/>
       <c r="Q81" s="10"/>
     </row>
-    <row r="82" spans="7:17" ht="12">
+    <row r="82" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G82" s="9"/>
       <c r="H82" s="23"/>
       <c r="I82" s="23"/>
       <c r="L82" s="9"/>
       <c r="Q82" s="10"/>
     </row>
-    <row r="83" spans="7:17" ht="12">
+    <row r="83" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G83" s="9"/>
       <c r="H83" s="23"/>
       <c r="I83" s="23"/>
       <c r="L83" s="9"/>
       <c r="Q83" s="10"/>
     </row>
-    <row r="84" spans="7:17" ht="12">
+    <row r="84" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G84" s="9"/>
       <c r="H84" s="23"/>
       <c r="I84" s="23"/>
       <c r="L84" s="9"/>
       <c r="Q84" s="10"/>
     </row>
-    <row r="85" spans="7:17" ht="12">
+    <row r="85" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G85" s="9"/>
       <c r="H85" s="23"/>
       <c r="I85" s="23"/>
       <c r="L85" s="9"/>
       <c r="Q85" s="10"/>
     </row>
-    <row r="86" spans="7:17" ht="12">
+    <row r="86" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G86" s="9"/>
       <c r="H86" s="23"/>
       <c r="I86" s="23"/>
       <c r="L86" s="9"/>
       <c r="Q86" s="10"/>
     </row>
-    <row r="87" spans="7:17" ht="12">
+    <row r="87" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G87" s="9"/>
       <c r="H87" s="23"/>
       <c r="I87" s="23"/>
       <c r="L87" s="9"/>
       <c r="Q87" s="10"/>
     </row>
-    <row r="88" spans="7:17" ht="12">
+    <row r="88" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G88" s="9"/>
       <c r="H88" s="23"/>
       <c r="I88" s="23"/>
       <c r="L88" s="9"/>
       <c r="Q88" s="10"/>
     </row>
-    <row r="89" spans="7:17" ht="12">
+    <row r="89" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G89" s="9"/>
       <c r="H89" s="23"/>
       <c r="I89" s="23"/>
       <c r="L89" s="9"/>
       <c r="Q89" s="10"/>
     </row>
-    <row r="90" spans="7:17" ht="12">
+    <row r="90" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G90" s="9"/>
       <c r="H90" s="23"/>
       <c r="I90" s="23"/>
       <c r="L90" s="9"/>
       <c r="Q90" s="10"/>
     </row>
-    <row r="91" spans="7:17" ht="12">
+    <row r="91" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G91" s="9"/>
       <c r="H91" s="23"/>
       <c r="I91" s="23"/>
       <c r="L91" s="9"/>
       <c r="Q91" s="10"/>
     </row>
-    <row r="92" spans="7:17" ht="12">
+    <row r="92" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G92" s="9"/>
       <c r="H92" s="23"/>
       <c r="I92" s="23"/>
       <c r="L92" s="9"/>
       <c r="Q92" s="10"/>
     </row>
-    <row r="93" spans="7:17" ht="12">
+    <row r="93" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G93" s="9"/>
       <c r="H93" s="23"/>
       <c r="I93" s="23"/>
       <c r="L93" s="9"/>
       <c r="Q93" s="10"/>
     </row>
-    <row r="94" spans="7:17" ht="12">
+    <row r="94" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G94" s="9"/>
       <c r="H94" s="23"/>
       <c r="I94" s="23"/>
       <c r="L94" s="9"/>
       <c r="Q94" s="10"/>
     </row>
-    <row r="95" spans="7:17" ht="12">
+    <row r="95" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G95" s="9"/>
       <c r="H95" s="23"/>
       <c r="I95" s="23"/>
       <c r="L95" s="9"/>
       <c r="Q95" s="10"/>
     </row>
-    <row r="96" spans="7:17" ht="12">
+    <row r="96" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G96" s="9"/>
       <c r="H96" s="23"/>
       <c r="I96" s="23"/>
       <c r="L96" s="9"/>
       <c r="Q96" s="10"/>
     </row>
-    <row r="97" spans="7:17" ht="12">
+    <row r="97" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G97" s="9"/>
       <c r="H97" s="23"/>
       <c r="I97" s="23"/>
       <c r="L97" s="9"/>
       <c r="Q97" s="10"/>
     </row>
-    <row r="98" spans="7:17" ht="12">
+    <row r="98" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G98" s="9"/>
       <c r="H98" s="23"/>
       <c r="I98" s="23"/>
       <c r="L98" s="9"/>
       <c r="Q98" s="10"/>
     </row>
-    <row r="99" spans="7:17" ht="12">
+    <row r="99" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G99" s="9"/>
       <c r="H99" s="23"/>
       <c r="I99" s="23"/>
       <c r="L99" s="9"/>
       <c r="Q99" s="10"/>
     </row>
-    <row r="100" spans="7:17" ht="12">
+    <row r="100" spans="7:17" x14ac:dyDescent="0.2">
       <c r="G100" s="9"/>
       <c r="H100" s="23"/>
       <c r="I100" s="23"/>

</xml_diff>